<commit_message>
Delete a Skill change
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="4950" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="14355" windowHeight="4950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SignUp" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>Url</t>
   </si>
@@ -202,13 +202,16 @@
     <t>PM</t>
   </si>
   <si>
+    <t xml:space="preserve">Best place to  accomplished your all the reading and translation needs.   </t>
+  </si>
+  <si>
+    <t>Delete record</t>
+  </si>
+  <si>
     <t>Writing No1</t>
   </si>
   <si>
-    <t xml:space="preserve">Best place to  accomplished your all the reading and translation needs.   </t>
-  </si>
-  <si>
-    <t>Delete record</t>
+    <t>Writing best</t>
   </si>
 </sst>
 </file>
@@ -272,7 +275,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
@@ -299,6 +302,9 @@
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -801,7 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -867,10 +873,10 @@
     </row>
     <row r="2" spans="1:17" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>37</v>
@@ -996,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,15 +1017,15 @@
         <v>34</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>59</v>
+      <c r="B2" s="15" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change of the Delete Manage Listing
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -208,10 +208,10 @@
     <t>Delete record</t>
   </si>
   <si>
+    <t>Writing qa</t>
+  </si>
+  <si>
     <t>Writing No1</t>
-  </si>
-  <si>
-    <t>Writing best</t>
   </si>
 </sst>
 </file>

</xml_diff>